<commit_message>
Changes in loginPage Event Class To check err
</commit_message>
<xml_diff>
--- a/datafiles/enduserdata1.xlsx
+++ b/datafiles/enduserdata1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{4C499F13-053C-40F8-A460-9BF713B56435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B12EC39-208C-4682-B9DC-929A822ED574}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{4C499F13-053C-40F8-A460-9BF713B56435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C682B680-11E5-469A-BF61-6984C61CD420}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="8">
   <si>
     <t>sethiya</t>
-  </si>
-  <si>
-    <t>Dinesh</t>
   </si>
   <si>
     <t>sethiya.dinesh@mailinator.com</t>
@@ -434,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -445,32 +442,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>8008008014</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D3" s="1"/>
@@ -482,9 +463,6 @@
       <c r="D5" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{CBEC7E8F-3BB1-4B0E-AC1B-8994CC99F733}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -493,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6CB5A1-397B-4F62-9904-7BF494C29275}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -501,21 +479,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -524,7 +502,7 @@
         <v>8008008014</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maven update, Jenkins Setup, Negative Cases for End User
</commit_message>
<xml_diff>
--- a/datafiles/enduserdata1.xlsx
+++ b/datafiles/enduserdata1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{4C499F13-053C-40F8-A460-9BF713B56435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C682B680-11E5-469A-BF61-6984C61CD420}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{4C499F13-053C-40F8-A460-9BF713B56435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76E087F4-7A2A-4F9B-81F4-0A6703AA710D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="7">
   <si>
     <t>sethiya</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>Mahesh</t>
   </si>
 </sst>
 </file>
@@ -431,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -471,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6CB5A1-397B-4F62-9904-7BF494C29275}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -492,9 +489,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Getting css error to select date from calender
</commit_message>
<xml_diff>
--- a/datafiles/enduserdata1.xlsx
+++ b/datafiles/enduserdata1.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{4C499F13-053C-40F8-A460-9BF713B56435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76E087F4-7A2A-4F9B-81F4-0A6703AA710D}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{4C499F13-053C-40F8-A460-9BF713B56435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8AF2A27-C81E-4B8B-9BED-3BBD2BD696BC}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>sethiya</t>
   </si>
@@ -45,13 +46,25 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>exDay</t>
+  </si>
+  <si>
+    <t>exMonth</t>
+  </si>
+  <si>
+    <t>exYear</t>
+  </si>
+  <si>
+    <t>JAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +94,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -103,7 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -111,6 +137,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6CB5A1-397B-4F62-9904-7BF494C29275}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -506,4 +538,41 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329D4C70-F440-4CEC-853B-C3F821B8091B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved stale element reference exception and Multiple Looping issue
</commit_message>
<xml_diff>
--- a/datafiles/enduserdata1.xlsx
+++ b/datafiles/enduserdata1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{4C499F13-053C-40F8-A460-9BF713B56435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8AF2A27-C81E-4B8B-9BED-3BBD2BD696BC}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{4C499F13-053C-40F8-A460-9BF713B56435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1ACBD37B-DE74-467D-BEE2-C83932CDDD1C}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="15">
   <si>
     <t>sethiya</t>
   </si>
@@ -58,13 +58,25 @@
   </si>
   <si>
     <t>JAN</t>
+  </si>
+  <si>
+    <t>exDay2</t>
+  </si>
+  <si>
+    <t>exMonth2</t>
+  </si>
+  <si>
+    <t>exYear2</t>
+  </si>
+  <si>
+    <t>JUL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +118,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -542,15 +560,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329D4C70-F440-4CEC-853B-C3F821B8091B}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -560,8 +578,17 @@
       <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>10</v>
       </c>
@@ -571,8 +598,18 @@
       <c r="C2" s="6">
         <v>2020</v>
       </c>
+      <c r="D2" s="6">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="6">
+        <v>2022</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" alignment="center"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FA 1843 finished few points remaining for code refactoring.
</commit_message>
<xml_diff>
--- a/datafiles/enduserdata1.xlsx
+++ b/datafiles/enduserdata1.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{4C499F13-053C-40F8-A460-9BF713B56435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1ACBD37B-DE74-467D-BEE2-C83932CDDD1C}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/IdeaProjects/FalconMain/datafiles/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88C32E4-5E22-9D40-810C-5974BA1FA443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="14800" windowHeight="8020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>sethiya</t>
   </si>
@@ -70,13 +76,34 @@
   </si>
   <si>
     <t>JUL</t>
+  </si>
+  <si>
+    <t>reportType</t>
+  </si>
+  <si>
+    <t>searchData</t>
+  </si>
+  <si>
+    <t>reportFilter</t>
+  </si>
+  <si>
+    <t>Users Details</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>pooja</t>
+  </si>
+  <si>
+    <t>First Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,18 +174,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -482,31 +508,28 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="14.390625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="D5" s="1"/>
     </row>
   </sheetData>
@@ -522,9 +545,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -538,15 +561,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <v>8008008014</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -562,49 +584,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329D4C70-F440-4CEC-853B-C3F821B8091B}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+    <row r="2" spans="1:6" ht="16">
+      <c r="A2" s="5">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>2020</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>2022</v>
       </c>
     </row>
@@ -612,4 +634,77 @@
   <phoneticPr fontId="6" alignment="center"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A110C0D7-A047-F942-A40A-CFD1A278798C}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>2021</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>2022</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Get error on Dart portal
</commit_message>
<xml_diff>
--- a/datafiles/enduserdata1.xlsx
+++ b/datafiles/enduserdata1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2946" uniqueCount="2857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2967" uniqueCount="2857">
   <si>
     <t>email</t>
   </si>
@@ -9047,7 +9047,7 @@
   <dimension ref="A1:D971"/>
   <sheetViews>
     <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D31"/>
+      <selection activeCell="A8" sqref="A8:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -22788,13 +22788,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
@@ -22839,22 +22843,102 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="A4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="6">
+        <v>9937332472</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="A5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3229586314</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4017474974</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="6">
+        <v>9886461734</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="6">
+        <v>6215280870</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3791890473</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1576046257</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>